<commit_message>
Actualizacion de riesgos y tiempos
</commit_message>
<xml_diff>
--- a/Seguimiento/Riesgos.xlsx
+++ b/Seguimiento/Riesgos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-630" yWindow="3510" windowWidth="20730" windowHeight="4380"/>
+    <workbookView xWindow="-630" yWindow="3570" windowWidth="20730" windowHeight="4320" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="R3" sheetId="7" r:id="rId1"/>
@@ -93,7 +93,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-sep15-sep21</t>
+sep15-sep21 Semana de trabajo individual</t>
         </r>
       </text>
     </comment>
@@ -1593,7 +1593,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="120">
   <si>
     <t>Código del riesgo</t>
   </si>
@@ -1930,10 +1930,31 @@
     <t xml:space="preserve">Hubo un error de comunicación que retraso un día el avance en el desarrollo del frontend (entresemana) . GM hizo limpieza de datos y considero que ya había dejado los datos como los necesitaba DA y FF, ya que fue notificado del error justo despues que realizo la operacion de liempieza.   </t>
   </si>
   <si>
-    <t xml:space="preserve">Comentarios </t>
-  </si>
-  <si>
     <t>Comentarios</t>
+  </si>
+  <si>
+    <t>Hemos tenido como medio de comunicación Skype, Hangouts y reuniones presenciales. Y como soportes de la comunicación documentación generada Alojada en Github y Google Drive</t>
+  </si>
+  <si>
+    <t>No fue necesario</t>
+  </si>
+  <si>
+    <t>El documento de integración siempre que se necesito,estuvo creado.</t>
+  </si>
+  <si>
+    <t>Establecer una charla entre los direactamente implicados</t>
+  </si>
+  <si>
+    <t>Hacer copias de seguridad de archivos criticos: SVN</t>
+  </si>
+  <si>
+    <t>Se realizo una copia del estado actual de los archivos importantes de las 3 máquinas</t>
+  </si>
+  <si>
+    <t>No se hizo el adecuado seguimiento de esta tarea, porque no se capacito al equipo en el uso de Tortoise, era algo complejo hacerle seguimiento a todos los repositorios, y al finalizar el ciclo (semana 5) hubo problemas de almacenamiento de los commit, probablemente se llego al topo de espacio permitido en el reporsitorio. Se manejo activamente para el proyecto de Sugarcallout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Realizar copias de seguridad preventivas </t>
   </si>
 </sst>
 </file>
@@ -2019,7 +2040,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2059,6 +2080,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2902,7 +2929,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="177">
+  <cellXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -3149,257 +3176,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
@@ -3412,11 +3193,267 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="158">
+  <dxfs count="200">
     <dxf>
       <fill>
         <patternFill>
@@ -3441,6 +3478,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -3455,6 +3499,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -3469,6 +3520,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -3483,6 +3541,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -3497,6 +3562,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -3532,6 +3604,76 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -3539,6 +3681,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
@@ -3546,6 +3695,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -4323,6 +4486,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -4337,6 +4507,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -4379,6 +4556,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
@@ -4393,6 +4577,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -4463,6 +4668,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -4470,6 +4689,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -4477,6 +4710,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -4499,6 +4746,90 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4822,8 +5153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4838,7 +5169,7 @@
     <col min="9" max="9" width="13.85546875" customWidth="1"/>
     <col min="10" max="11" width="16" customWidth="1"/>
     <col min="12" max="17" width="0" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" style="174" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" style="92" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -4857,52 +5188,52 @@
       <c r="E1" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="175" t="s">
+      <c r="F1" s="93" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="176" t="s">
+      <c r="G1" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="176" t="s">
+      <c r="H1" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="176" t="s">
+      <c r="I1" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="176" t="s">
+      <c r="J1" s="94" t="s">
         <v>107</v>
       </c>
-      <c r="K1" s="176" t="s">
+      <c r="K1" s="94" t="s">
         <v>105</v>
       </c>
-      <c r="L1" s="176" t="s">
+      <c r="L1" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="176" t="s">
+      <c r="M1" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="176" t="s">
+      <c r="N1" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="176" t="s">
+      <c r="O1" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="175" t="s">
+      <c r="P1" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="175" t="s">
+      <c r="Q1" s="93" t="s">
         <v>106</v>
       </c>
-      <c r="R1" s="172" t="s">
-        <v>112</v>
+      <c r="R1" s="90" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="str">
+      <c r="A2" s="95" t="str">
         <f>'Detalles plan de riesgo'!A2:A6</f>
         <v>R3</v>
       </c>
-      <c r="B2" s="91" t="str">
+      <c r="B2" s="98" t="str">
         <f>'Detalles plan de riesgo'!B2:B6</f>
         <v>El tiempo gastado para llevar a cabo cada una de las actividades del proyecto es superior al planeado</v>
       </c>
@@ -4910,7 +5241,7 @@
         <f>'Detalles plan de riesgo'!F2</f>
         <v>Hacer un seguimiento continuo (semanal) al cronograma.</v>
       </c>
-      <c r="D2" s="99"/>
+      <c r="D2" s="106"/>
       <c r="E2" s="80" t="s">
         <v>94</v>
       </c>
@@ -4928,19 +5259,18 @@
       <c r="O2" s="54"/>
       <c r="P2" s="61"/>
       <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
       <c r="S2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="51" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="92"/>
+      <c r="A3" s="96"/>
+      <c r="B3" s="99"/>
       <c r="C3" s="74" t="str">
         <f>'Detalles plan de riesgo'!F3</f>
         <v xml:space="preserve">Hacer un registro continuo de tiempos por parte de cada integrante. </v>
       </c>
-      <c r="D3" s="100"/>
+      <c r="D3" s="107"/>
       <c r="E3" s="81" t="s">
         <v>95</v>
       </c>
@@ -4948,7 +5278,9 @@
         <v>77</v>
       </c>
       <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
+      <c r="H3" s="55" t="s">
+        <v>77</v>
+      </c>
       <c r="I3" s="55" t="s">
         <v>77</v>
       </c>
@@ -4962,22 +5294,21 @@
       <c r="O3" s="55"/>
       <c r="P3" s="62"/>
       <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
       <c r="S3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="89"/>
-      <c r="B4" s="92"/>
-      <c r="C4" s="97" t="str">
+      <c r="A4" s="96"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="104" t="str">
         <f>'Detalles plan de riesgo'!F4</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D4" s="75" t="s">
         <v>104</v>
       </c>
-      <c r="E4" s="101"/>
+      <c r="E4" s="108"/>
       <c r="F4" s="62" t="s">
         <v>47</v>
       </c>
@@ -4994,16 +5325,15 @@
       <c r="O4" s="55"/>
       <c r="P4" s="62"/>
       <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="89"/>
-      <c r="B5" s="92"/>
-      <c r="C5" s="97"/>
+      <c r="A5" s="96"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="104"/>
       <c r="D5" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="101"/>
+      <c r="E5" s="108"/>
       <c r="F5" s="62" t="s">
         <v>49</v>
       </c>
@@ -5018,19 +5348,18 @@
       <c r="O5" s="55"/>
       <c r="P5" s="62"/>
       <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
       <c r="S5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="89"/>
-      <c r="B6" s="92"/>
-      <c r="C6" s="97"/>
+      <c r="A6" s="96"/>
+      <c r="B6" s="99"/>
+      <c r="C6" s="104"/>
       <c r="D6" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="101"/>
+      <c r="E6" s="108"/>
       <c r="F6" s="62" t="s">
         <v>49</v>
       </c>
@@ -5045,16 +5374,15 @@
       <c r="O6" s="55"/>
       <c r="P6" s="62"/>
       <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
     </row>
     <row r="7" spans="1:19" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="89"/>
-      <c r="B7" s="93"/>
-      <c r="C7" s="98"/>
+      <c r="A7" s="96"/>
+      <c r="B7" s="100"/>
+      <c r="C7" s="105"/>
       <c r="D7" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="102"/>
+      <c r="E7" s="109"/>
       <c r="F7" s="62" t="s">
         <v>49</v>
       </c>
@@ -5069,16 +5397,15 @@
       <c r="O7" s="55"/>
       <c r="P7" s="62"/>
       <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
     </row>
     <row r="8" spans="1:19" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="90"/>
-      <c r="B8" s="94" t="s">
+      <c r="A8" s="97"/>
+      <c r="B8" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="95"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="96"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="103"/>
       <c r="F8" s="72" t="s">
         <v>75</v>
       </c>
@@ -5096,8 +5423,7 @@
       <c r="N8" s="56"/>
       <c r="O8" s="56"/>
       <c r="P8" s="65"/>
-      <c r="Q8" s="173"/>
-      <c r="R8" s="173"/>
+      <c r="Q8" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -5108,67 +5434,67 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E4:E7"/>
   </mergeCells>
-  <conditionalFormatting sqref="G2:R7 D2 F8:R8 D4">
-    <cfRule type="cellIs" dxfId="157" priority="12" operator="equal">
+  <conditionalFormatting sqref="D2 F8:Q8 D4 G2:Q7">
+    <cfRule type="cellIs" dxfId="187" priority="12" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="13" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2 G2:R4">
-    <cfRule type="cellIs" dxfId="155" priority="11" operator="equal">
+  <conditionalFormatting sqref="D2 G2:Q4">
+    <cfRule type="cellIs" dxfId="185" priority="11" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="cellIs" dxfId="154" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="10" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5:R7">
-    <cfRule type="cellIs" dxfId="153" priority="9" operator="equal">
+  <conditionalFormatting sqref="G5:Q7">
+    <cfRule type="cellIs" dxfId="183" priority="9" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F7">
-    <cfRule type="cellIs" dxfId="152" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="7" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="8" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="150" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="6" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F4">
-    <cfRule type="cellIs" dxfId="149" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="5" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F7">
-    <cfRule type="cellIs" dxfId="148" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="4" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E4">
-    <cfRule type="cellIs" dxfId="147" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="2" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="3" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="145" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="1" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:R7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:Q7">
       <formula1>$S$2:$S$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -5182,9 +5508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5199,7 +5523,7 @@
     <col min="10" max="10" width="16.7109375" customWidth="1"/>
     <col min="11" max="11" width="20.140625" customWidth="1"/>
     <col min="12" max="17" width="0" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" style="174" customWidth="1"/>
+    <col min="18" max="18" width="37.140625" style="92" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.3">
@@ -5218,51 +5542,51 @@
       <c r="E1" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="175" t="s">
+      <c r="F1" s="93" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="176" t="s">
+      <c r="G1" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="176" t="s">
+      <c r="H1" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="176" t="s">
+      <c r="I1" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="176" t="s">
+      <c r="J1" s="94" t="s">
         <v>107</v>
       </c>
-      <c r="K1" s="176" t="s">
+      <c r="K1" s="94" t="s">
         <v>105</v>
       </c>
-      <c r="L1" s="176" t="s">
+      <c r="L1" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="176" t="s">
+      <c r="M1" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="176" t="s">
+      <c r="N1" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="176" t="s">
+      <c r="O1" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="175" t="s">
+      <c r="P1" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="175" t="s">
+      <c r="Q1" s="93" t="s">
         <v>106</v>
       </c>
-      <c r="R1" s="172" t="s">
+      <c r="R1" s="90" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="110" t="s">
         <v>50</v>
       </c>
       <c r="C2" s="78" t="s">
@@ -5285,52 +5609,63 @@
       <c r="J2" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="54"/>
+      <c r="K2" s="54" t="s">
+        <v>47</v>
+      </c>
       <c r="L2" s="54"/>
       <c r="M2" s="54"/>
       <c r="N2" s="54"/>
       <c r="O2" s="54"/>
       <c r="P2" s="61"/>
       <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
+      <c r="R2" s="92" t="s">
+        <v>112</v>
+      </c>
       <c r="S2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="104"/>
-      <c r="C3" s="74" t="str">
-        <f>'Detalles plan de riesgo'!F2</f>
-        <v>Hacer un seguimiento continuo (semanal) al cronograma.</v>
+      <c r="A3" s="96"/>
+      <c r="B3" s="111"/>
+      <c r="C3" s="74" t="s">
+        <v>58</v>
       </c>
       <c r="D3" s="75"/>
       <c r="E3" s="81"/>
       <c r="F3" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
+      <c r="G3" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="55" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" s="55" t="s">
+        <v>47</v>
+      </c>
       <c r="L3" s="55"/>
       <c r="M3" s="55"/>
       <c r="N3" s="55"/>
       <c r="O3" s="55"/>
       <c r="P3" s="62"/>
       <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
       <c r="S3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="89"/>
-      <c r="B4" s="104"/>
-      <c r="C4" s="74" t="str">
-        <f>'Detalles plan de riesgo'!F3</f>
-        <v xml:space="preserve">Hacer un registro continuo de tiempos por parte de cada integrante. </v>
+    <row r="4" spans="1:19" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="96"/>
+      <c r="B4" s="111"/>
+      <c r="C4" s="74" t="s">
+        <v>84</v>
       </c>
       <c r="D4" s="75"/>
       <c r="E4" s="81" t="s">
@@ -5339,22 +5674,37 @@
       <c r="F4" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
+      <c r="G4" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="J4" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" s="55" t="s">
+        <v>77</v>
+      </c>
       <c r="L4" s="55"/>
       <c r="M4" s="55"/>
       <c r="N4" s="55"/>
       <c r="O4" s="55"/>
       <c r="P4" s="62"/>
       <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
+      <c r="R4" s="179" t="s">
+        <v>114</v>
+      </c>
+      <c r="S4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="5" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="89"/>
-      <c r="B5" s="104"/>
+      <c r="A5" s="96"/>
+      <c r="B5" s="111"/>
       <c r="C5" s="74" t="str">
         <f>'Detalles plan de riesgo'!F4</f>
         <v xml:space="preserve"> </v>
@@ -5366,53 +5716,75 @@
       <c r="F5" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="55"/>
+      <c r="G5" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="J5" s="180" t="s">
+        <v>113</v>
+      </c>
+      <c r="K5" s="55" t="s">
+        <v>49</v>
+      </c>
       <c r="L5" s="55"/>
       <c r="M5" s="55"/>
       <c r="N5" s="55"/>
       <c r="O5" s="55"/>
       <c r="P5" s="62"/>
       <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
       <c r="S5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="89"/>
-      <c r="B6" s="104"/>
+    <row r="6" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="96"/>
+      <c r="B6" s="111"/>
       <c r="C6" s="74" t="str">
         <f>'Detalles plan de riesgo'!F5</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D6" s="25"/>
+      <c r="D6" s="88" t="s">
+        <v>115</v>
+      </c>
       <c r="E6" s="81"/>
-      <c r="F6" s="62"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
+      <c r="F6" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="J6" s="180" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="55" t="s">
+        <v>49</v>
+      </c>
       <c r="L6" s="55"/>
       <c r="M6" s="55"/>
       <c r="N6" s="55"/>
       <c r="O6" s="55"/>
       <c r="P6" s="62"/>
       <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
     </row>
     <row r="7" spans="1:19" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="90"/>
-      <c r="B7" s="105" t="s">
+      <c r="A7" s="97"/>
+      <c r="B7" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="93"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="106"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="113"/>
       <c r="F7" s="72" t="s">
         <v>76</v>
       </c>
@@ -5428,8 +5800,7 @@
       <c r="N7" s="56"/>
       <c r="O7" s="56"/>
       <c r="P7" s="65"/>
-      <c r="Q7" s="173"/>
-      <c r="R7" s="173"/>
+      <c r="Q7" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5437,76 +5808,128 @@
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="B7:E7"/>
   </mergeCells>
-  <conditionalFormatting sqref="D6 H5:R5 G2:R4 F6:R7">
-    <cfRule type="cellIs" dxfId="144" priority="15" operator="equal">
+  <conditionalFormatting sqref="G2:Q4 F7:Q7 L5:Q6">
+    <cfRule type="cellIs" dxfId="174" priority="27" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="28" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6 H5:R5 G2:R4 F6:R6">
-    <cfRule type="cellIs" dxfId="142" priority="14" operator="equal">
+  <conditionalFormatting sqref="G2:Q4 L5:Q6">
+    <cfRule type="cellIs" dxfId="172" priority="26" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="141" priority="12" operator="equal">
+  <conditionalFormatting sqref="G5:G6">
+    <cfRule type="cellIs" dxfId="171" priority="24" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="25" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="139" priority="11" operator="equal">
+  <conditionalFormatting sqref="G5:G6">
+    <cfRule type="cellIs" dxfId="169" priority="23" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F4">
-    <cfRule type="cellIs" dxfId="138" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="21" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="22" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F4">
-    <cfRule type="cellIs" dxfId="136" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="20" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="135" priority="6" operator="equal">
+  <conditionalFormatting sqref="F5:F6">
+    <cfRule type="cellIs" dxfId="165" priority="18" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="19" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="133" priority="5" operator="equal">
+  <conditionalFormatting sqref="F5:F6">
+    <cfRule type="cellIs" dxfId="163" priority="17" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D4">
-    <cfRule type="cellIs" dxfId="132" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="15" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="16" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E6">
-    <cfRule type="cellIs" dxfId="130" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="13" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="14" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H5:H6">
+    <cfRule type="cellIs" dxfId="158" priority="11" operator="equal">
+      <formula>$S$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="157" priority="12" operator="equal">
+      <formula>$S$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5:H6">
+    <cfRule type="cellIs" dxfId="156" priority="10" operator="equal">
+      <formula>$S$5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5:I6">
+    <cfRule type="cellIs" dxfId="155" priority="8" operator="equal">
+      <formula>$S$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="154" priority="9" operator="equal">
+      <formula>$S$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5:I6">
+    <cfRule type="cellIs" dxfId="153" priority="7" operator="equal">
+      <formula>$S$5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:J6">
+    <cfRule type="cellIs" dxfId="152" priority="5" operator="equal">
+      <formula>$S$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="151" priority="6" operator="equal">
+      <formula>$S$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5:J6">
+    <cfRule type="cellIs" dxfId="150" priority="4" operator="equal">
+      <formula>$S$5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5:K6">
+    <cfRule type="cellIs" dxfId="149" priority="2" operator="equal">
+      <formula>$S$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="148" priority="3" operator="equal">
+      <formula>$S$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5:K6">
+    <cfRule type="cellIs" dxfId="147" priority="1" operator="equal">
+      <formula>$S$5</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 F2:R6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:Q6">
       <formula1>$S$2:$S$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -5520,14 +5943,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
     <col min="12" max="17" width="0" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="174"/>
+    <col min="18" max="18" width="33.5703125" style="92" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5546,54 +5974,55 @@
       <c r="E1" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="175" t="s">
+      <c r="F1" s="93" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="176" t="s">
+      <c r="G1" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="176" t="s">
+      <c r="H1" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="176" t="s">
+      <c r="I1" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="176" t="s">
+      <c r="J1" s="94" t="s">
         <v>107</v>
       </c>
-      <c r="K1" s="176" t="s">
+      <c r="K1" s="94" t="s">
         <v>105</v>
       </c>
-      <c r="L1" s="176" t="s">
+      <c r="L1" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="176" t="s">
+      <c r="M1" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="176" t="s">
+      <c r="N1" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="176" t="s">
+      <c r="O1" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="175" t="s">
+      <c r="P1" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="175" t="s">
+      <c r="Q1" s="93" t="s">
         <v>106</v>
       </c>
-      <c r="R1" s="172"/>
+      <c r="R1" s="90" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="2" spans="1:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="110" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="78" t="str">
-        <f>'Detalles plan de riesgo'!F1</f>
-        <v>Respuestas Planificadas</v>
+      <c r="C2" s="78" t="s">
+        <v>60</v>
       </c>
       <c r="D2" s="79"/>
       <c r="E2" s="80"/>
@@ -5611,17 +6040,15 @@
       <c r="O2" s="54"/>
       <c r="P2" s="61"/>
       <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
       <c r="S2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="104"/>
-      <c r="C3" s="74" t="str">
-        <f>'Detalles plan de riesgo'!F2</f>
-        <v>Hacer un seguimiento continuo (semanal) al cronograma.</v>
+    <row r="3" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="96"/>
+      <c r="B3" s="111"/>
+      <c r="C3" s="74" t="s">
+        <v>64</v>
       </c>
       <c r="D3" s="75"/>
       <c r="E3" s="81" t="s">
@@ -5630,29 +6057,38 @@
       <c r="F3" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
+      <c r="G3" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" s="55" t="s">
+        <v>77</v>
+      </c>
+      <c r="K3" s="55" t="s">
+        <v>77</v>
+      </c>
       <c r="L3" s="55"/>
       <c r="M3" s="55"/>
       <c r="N3" s="55"/>
       <c r="O3" s="55"/>
       <c r="P3" s="62"/>
       <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
+      <c r="R3" s="146" t="s">
+        <v>118</v>
+      </c>
       <c r="S3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="89"/>
-      <c r="B4" s="104"/>
-      <c r="C4" s="74" t="str">
-        <f>'Detalles plan de riesgo'!F3</f>
-        <v xml:space="preserve">Hacer un registro continuo de tiempos por parte de cada integrante. </v>
-      </c>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="96"/>
+      <c r="B4" s="111"/>
+      <c r="C4" s="74"/>
       <c r="D4" s="75"/>
       <c r="E4" s="81"/>
       <c r="F4" s="62"/>
@@ -5667,19 +6103,16 @@
       <c r="O4" s="55"/>
       <c r="P4" s="62"/>
       <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
-    </row>
-    <row r="5" spans="1:19" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="89"/>
-      <c r="B5" s="104"/>
+      <c r="R4" s="146"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="96"/>
+      <c r="B5" s="111"/>
       <c r="C5" s="74" t="str">
         <f>'Detalles plan de riesgo'!F4</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D5" s="74" t="str">
-        <f>'Detalles plan de riesgo'!G4</f>
-        <v xml:space="preserve"> Contingencia</v>
-      </c>
+      <c r="D5" s="74"/>
       <c r="E5" s="81"/>
       <c r="F5" s="73"/>
       <c r="G5" s="55"/>
@@ -5693,14 +6126,14 @@
       <c r="O5" s="55"/>
       <c r="P5" s="62"/>
       <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
+      <c r="R5" s="146"/>
       <c r="S5" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="51" x14ac:dyDescent="0.25">
-      <c r="A6" s="89"/>
-      <c r="B6" s="104"/>
+    <row r="6" spans="1:19" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="96"/>
+      <c r="B6" s="111"/>
       <c r="C6" s="74" t="str">
         <f>'Detalles plan de riesgo'!F5</f>
         <v xml:space="preserve"> </v>
@@ -5723,17 +6156,18 @@
       <c r="O6" s="55"/>
       <c r="P6" s="62"/>
       <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
-    </row>
-    <row r="7" spans="1:19" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="90"/>
-      <c r="B7" s="105" t="s">
+    </row>
+    <row r="7" spans="1:19" ht="132" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="97"/>
+      <c r="B7" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="93"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="106"/>
-      <c r="F7" s="65"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="72" t="s">
+        <v>117</v>
+      </c>
       <c r="G7" s="56"/>
       <c r="H7" s="56"/>
       <c r="I7" s="56"/>
@@ -5744,93 +6178,93 @@
       <c r="N7" s="56"/>
       <c r="O7" s="56"/>
       <c r="P7" s="65"/>
-      <c r="Q7" s="173"/>
-      <c r="R7" s="173"/>
+      <c r="Q7" s="91"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="B7:E7"/>
+    <mergeCell ref="R3:R5"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:R6">
-    <cfRule type="cellIs" dxfId="128" priority="17" operator="equal">
+  <conditionalFormatting sqref="H5:Q6">
+    <cfRule type="cellIs" dxfId="146" priority="17" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="18" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7:R7">
-    <cfRule type="cellIs" dxfId="126" priority="15" operator="equal">
+  <conditionalFormatting sqref="F7:Q7">
+    <cfRule type="cellIs" dxfId="144" priority="15" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="16" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:R6">
-    <cfRule type="cellIs" dxfId="124" priority="14" operator="equal">
+  <conditionalFormatting sqref="H5:Q6">
+    <cfRule type="cellIs" dxfId="142" priority="14" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:R4">
-    <cfRule type="cellIs" dxfId="123" priority="12" operator="equal">
+  <conditionalFormatting sqref="F2:Q4">
+    <cfRule type="cellIs" dxfId="141" priority="12" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="13" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:R4">
-    <cfRule type="cellIs" dxfId="121" priority="11" operator="equal">
+  <conditionalFormatting sqref="F2:Q4">
+    <cfRule type="cellIs" dxfId="139" priority="11" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G6">
-    <cfRule type="cellIs" dxfId="120" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="9" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="10" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G6">
-    <cfRule type="cellIs" dxfId="118" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="8" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="117" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="6" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="7" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="115" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="5" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D4">
-    <cfRule type="cellIs" dxfId="114" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="3" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="4" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E6">
-    <cfRule type="cellIs" dxfId="112" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="1" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="2" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6 F2:F4 G2:R6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6 F2:F4 G2:Q6">
       <formula1>$S$2:$S$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -5844,14 +6278,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
     <col min="12" max="17" width="0" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="174"/>
+    <col min="18" max="18" width="12.85546875" style="92" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5870,49 +6312,51 @@
       <c r="E1" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="175" t="s">
+      <c r="F1" s="93" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="176" t="s">
+      <c r="G1" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="176" t="s">
+      <c r="H1" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="176" t="s">
+      <c r="I1" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="176" t="s">
+      <c r="J1" s="94" t="s">
         <v>107</v>
       </c>
-      <c r="K1" s="176" t="s">
+      <c r="K1" s="94" t="s">
         <v>105</v>
       </c>
-      <c r="L1" s="176" t="s">
+      <c r="L1" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="176" t="s">
+      <c r="M1" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="176" t="s">
+      <c r="N1" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="176" t="s">
+      <c r="O1" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="175" t="s">
+      <c r="P1" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="175" t="s">
+      <c r="Q1" s="93" t="s">
         <v>106</v>
       </c>
-      <c r="R1" s="172"/>
+      <c r="R1" s="90" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="2" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="110" t="s">
         <v>51</v>
       </c>
       <c r="C2" s="78" t="str">
@@ -5937,14 +6381,13 @@
       <c r="O2" s="54"/>
       <c r="P2" s="61"/>
       <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
       <c r="S2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="104"/>
+      <c r="A3" s="96"/>
+      <c r="B3" s="111"/>
       <c r="C3" s="74" t="str">
         <f>'Detalles plan de riesgo'!F2</f>
         <v>Hacer un seguimiento continuo (semanal) al cronograma.</v>
@@ -5967,14 +6410,13 @@
       <c r="O3" s="55"/>
       <c r="P3" s="62"/>
       <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
       <c r="S3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="89"/>
-      <c r="B4" s="104"/>
+      <c r="A4" s="96"/>
+      <c r="B4" s="111"/>
       <c r="C4" s="74" t="str">
         <f>'Detalles plan de riesgo'!F3</f>
         <v xml:space="preserve">Hacer un registro continuo de tiempos por parte de cada integrante. </v>
@@ -5995,11 +6437,10 @@
       <c r="O4" s="55"/>
       <c r="P4" s="62"/>
       <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
     </row>
     <row r="5" spans="1:19" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" s="89"/>
-      <c r="B5" s="104"/>
+      <c r="A5" s="96"/>
+      <c r="B5" s="111"/>
       <c r="C5" s="74" t="str">
         <f>'Detalles plan de riesgo'!F4</f>
         <v xml:space="preserve"> </v>
@@ -6022,14 +6463,13 @@
       <c r="O5" s="55"/>
       <c r="P5" s="62"/>
       <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
       <c r="S5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="89"/>
-      <c r="B6" s="104"/>
+      <c r="A6" s="96"/>
+      <c r="B6" s="111"/>
       <c r="C6" s="74" t="str">
         <f>'Detalles plan de riesgo'!F5</f>
         <v xml:space="preserve"> </v>
@@ -6052,14 +6492,13 @@
       <c r="O6" s="55"/>
       <c r="P6" s="62"/>
       <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
     </row>
     <row r="7" spans="1:19" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="90"/>
-      <c r="B7" s="105" t="s">
+      <c r="A7" s="97"/>
+      <c r="B7" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="93"/>
+      <c r="C7" s="100"/>
       <c r="D7" s="85"/>
       <c r="E7" s="83"/>
       <c r="F7" s="65"/>
@@ -6073,8 +6512,7 @@
       <c r="N7" s="56"/>
       <c r="O7" s="56"/>
       <c r="P7" s="65"/>
-      <c r="Q7" s="173"/>
-      <c r="R7" s="173"/>
+      <c r="Q7" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6082,84 +6520,84 @@
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="B7:C7"/>
   </mergeCells>
-  <conditionalFormatting sqref="D5:D6 H5:R6 G2:R4 F7:R7">
-    <cfRule type="cellIs" dxfId="110" priority="17" operator="equal">
+  <conditionalFormatting sqref="D5:D6 H5:Q6 G2:Q4 F7:Q7">
+    <cfRule type="cellIs" dxfId="128" priority="17" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="18" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="cellIs" dxfId="108" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="15" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="16" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D6 H5:R6 G2:R4">
-    <cfRule type="cellIs" dxfId="106" priority="14" operator="equal">
+  <conditionalFormatting sqref="D5:D6 H5:Q6 G2:Q4">
+    <cfRule type="cellIs" dxfId="124" priority="14" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G6">
-    <cfRule type="cellIs" dxfId="105" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="12" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="13" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G6">
-    <cfRule type="cellIs" dxfId="103" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="11" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F4">
-    <cfRule type="cellIs" dxfId="102" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="9" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="10" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F4">
-    <cfRule type="cellIs" dxfId="100" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="8" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F6">
-    <cfRule type="cellIs" dxfId="99" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="6" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="7" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F6">
-    <cfRule type="cellIs" dxfId="97" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="5" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D4">
-    <cfRule type="cellIs" dxfId="96" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="3" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="4" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E7">
-    <cfRule type="cellIs" dxfId="94" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="1" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="2" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D6 F2:R6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D6 F2:Q6">
       <formula1>$S$2:$S$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -6174,13 +6612,13 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="12" max="17" width="0" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="174"/>
+    <col min="18" max="18" width="12.85546875" style="92" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6199,54 +6637,55 @@
       <c r="E1" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="F1" s="175" t="s">
+      <c r="F1" s="93" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="176" t="s">
+      <c r="G1" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="176" t="s">
+      <c r="H1" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="176" t="s">
+      <c r="I1" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="176" t="s">
+      <c r="J1" s="94" t="s">
         <v>107</v>
       </c>
-      <c r="K1" s="176" t="s">
+      <c r="K1" s="94" t="s">
         <v>105</v>
       </c>
-      <c r="L1" s="176" t="s">
+      <c r="L1" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="M1" s="176" t="s">
+      <c r="M1" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="176" t="s">
+      <c r="N1" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="176" t="s">
+      <c r="O1" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="175" t="s">
+      <c r="P1" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="175" t="s">
+      <c r="Q1" s="93" t="s">
         <v>106</v>
       </c>
-      <c r="R1" s="172"/>
-    </row>
-    <row r="2" spans="1:19" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="s">
+      <c r="R1" s="90" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="110" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="78" t="str">
-        <f>'Detalles plan de riesgo'!F1</f>
-        <v>Respuestas Planificadas</v>
+      <c r="C2" s="78" t="s">
+        <v>116</v>
       </c>
       <c r="D2" s="79"/>
       <c r="E2" s="80" t="s">
@@ -6266,14 +6705,13 @@
       <c r="O2" s="54"/>
       <c r="P2" s="61"/>
       <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
       <c r="S2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="105" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="104"/>
+      <c r="A3" s="96"/>
+      <c r="B3" s="111"/>
       <c r="C3" s="74" t="str">
         <f>'Detalles plan de riesgo'!F2</f>
         <v>Hacer un seguimiento continuo (semanal) al cronograma.</v>
@@ -6296,14 +6734,13 @@
       <c r="O3" s="55"/>
       <c r="P3" s="62"/>
       <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
       <c r="S3" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="89"/>
-      <c r="B4" s="104"/>
+      <c r="A4" s="96"/>
+      <c r="B4" s="111"/>
       <c r="C4" s="74" t="str">
         <f>'Detalles plan de riesgo'!F3</f>
         <v xml:space="preserve">Hacer un registro continuo de tiempos por parte de cada integrante. </v>
@@ -6326,11 +6763,10 @@
       <c r="O4" s="55"/>
       <c r="P4" s="62"/>
       <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
     </row>
     <row r="5" spans="1:19" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="89"/>
-      <c r="B5" s="104"/>
+      <c r="A5" s="96"/>
+      <c r="B5" s="111"/>
       <c r="C5" s="74" t="str">
         <f>'Detalles plan de riesgo'!F4</f>
         <v xml:space="preserve"> </v>
@@ -6353,14 +6789,13 @@
       <c r="O5" s="55"/>
       <c r="P5" s="62"/>
       <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
       <c r="S5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="89"/>
-      <c r="B6" s="104"/>
+      <c r="A6" s="96"/>
+      <c r="B6" s="111"/>
       <c r="C6" s="74" t="str">
         <f>'Detalles plan de riesgo'!F5</f>
         <v xml:space="preserve"> </v>
@@ -6379,14 +6814,13 @@
       <c r="O6" s="55"/>
       <c r="P6" s="62"/>
       <c r="Q6" s="25"/>
-      <c r="R6" s="25"/>
     </row>
     <row r="7" spans="1:19" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="90"/>
-      <c r="B7" s="105" t="s">
+      <c r="A7" s="97"/>
+      <c r="B7" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="93"/>
+      <c r="C7" s="100"/>
       <c r="D7" s="84"/>
       <c r="E7" s="83"/>
       <c r="F7" s="65"/>
@@ -6400,8 +6834,7 @@
       <c r="N7" s="56"/>
       <c r="O7" s="56"/>
       <c r="P7" s="65"/>
-      <c r="Q7" s="173"/>
-      <c r="R7" s="173"/>
+      <c r="Q7" s="91"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6409,105 +6842,105 @@
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="B7:C7"/>
   </mergeCells>
-  <conditionalFormatting sqref="F6 H4:R6 D4:D5 G2:R3">
-    <cfRule type="cellIs" dxfId="92" priority="22" operator="equal">
+  <conditionalFormatting sqref="F6 H4:Q6 D4:D5 G2:Q3">
+    <cfRule type="cellIs" dxfId="110" priority="22" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="23" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7:R7">
-    <cfRule type="cellIs" dxfId="90" priority="20" operator="equal">
+  <conditionalFormatting sqref="F7:Q7">
+    <cfRule type="cellIs" dxfId="108" priority="20" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="21" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6 H4:R6 D4:D5 G2:R3">
-    <cfRule type="cellIs" dxfId="88" priority="19" operator="equal">
+  <conditionalFormatting sqref="F6 H4:Q6 D4:D5 G2:Q3">
+    <cfRule type="cellIs" dxfId="106" priority="19" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="87" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="17" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="18" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="85" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="16" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G6">
-    <cfRule type="cellIs" dxfId="84" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="14" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="15" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G6">
-    <cfRule type="cellIs" dxfId="82" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="13" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F3">
-    <cfRule type="cellIs" dxfId="81" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="11" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="12" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F3">
-    <cfRule type="cellIs" dxfId="79" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="10" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F5">
-    <cfRule type="cellIs" dxfId="78" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="8" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="9" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4:F5">
-    <cfRule type="cellIs" dxfId="76" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="7" operator="equal">
       <formula>$S$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="75" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="5" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="6" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:D7">
-    <cfRule type="cellIs" dxfId="73" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="3" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="4" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E7">
-    <cfRule type="cellIs" dxfId="71" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="1" operator="equal">
       <formula>$S$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="2" operator="equal">
       <formula>$S$2</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D5 F2:R6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D5 F2:Q6">
       <formula1>$S$2:$S$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -6520,8 +6953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6578,19 +7011,19 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="119" t="s">
+      <c r="A2" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="166" t="s">
+      <c r="B2" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="169" t="s">
+      <c r="C2" s="122" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="119" t="s">
+      <c r="D2" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="119">
+      <c r="E2" s="114">
         <v>3</v>
       </c>
       <c r="F2" s="57" t="s">
@@ -6614,16 +7047,16 @@
       <c r="L2" s="2">
         <v>9</v>
       </c>
-      <c r="M2" s="119" t="s">
+      <c r="M2" s="114" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="120"/>
-      <c r="B3" s="167"/>
-      <c r="C3" s="170"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="120"/>
+      <c r="A3" s="115"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
       <c r="F3" s="58" t="s">
         <v>54</v>
       </c>
@@ -6643,14 +7076,14 @@
       <c r="L3" s="2">
         <v>3</v>
       </c>
-      <c r="M3" s="120"/>
+      <c r="M3" s="115"/>
     </row>
     <row r="4" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="120"/>
-      <c r="B4" s="167"/>
-      <c r="C4" s="170"/>
-      <c r="D4" s="120"/>
-      <c r="E4" s="120"/>
+      <c r="A4" s="115"/>
+      <c r="B4" s="120"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="115"/>
       <c r="F4" s="9" t="s">
         <v>52</v>
       </c>
@@ -6672,14 +7105,14 @@
       <c r="L4" s="2">
         <v>6</v>
       </c>
-      <c r="M4" s="120"/>
+      <c r="M4" s="115"/>
     </row>
     <row r="5" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="120"/>
-      <c r="B5" s="167"/>
-      <c r="C5" s="170"/>
-      <c r="D5" s="120"/>
-      <c r="E5" s="120"/>
+      <c r="A5" s="115"/>
+      <c r="B5" s="120"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="115"/>
+      <c r="E5" s="115"/>
       <c r="F5" s="9" t="s">
         <v>52</v>
       </c>
@@ -6701,14 +7134,14 @@
       <c r="L5" s="2">
         <v>9</v>
       </c>
-      <c r="M5" s="120"/>
+      <c r="M5" s="115"/>
     </row>
     <row r="6" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="121"/>
-      <c r="B6" s="168"/>
-      <c r="C6" s="171"/>
-      <c r="D6" s="121"/>
-      <c r="E6" s="121"/>
+      <c r="A6" s="116"/>
+      <c r="B6" s="121"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="116"/>
+      <c r="E6" s="116"/>
       <c r="F6" s="10" t="s">
         <v>52</v>
       </c>
@@ -6728,7 +7161,7 @@
       <c r="L6" s="5">
         <v>27</v>
       </c>
-      <c r="M6" s="121"/>
+      <c r="M6" s="116"/>
     </row>
     <row r="7" spans="1:13" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="22" t="s">
@@ -6740,33 +7173,33 @@
       <c r="C7" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="122" t="s">
+      <c r="D7" s="117" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="123"/>
-      <c r="F7" s="123"/>
-      <c r="G7" s="123"/>
-      <c r="H7" s="123"/>
-      <c r="I7" s="123"/>
+      <c r="E7" s="118"/>
+      <c r="F7" s="118"/>
+      <c r="G7" s="118"/>
+      <c r="H7" s="118"/>
+      <c r="I7" s="118"/>
       <c r="J7" s="50"/>
       <c r="K7" s="50"/>
       <c r="L7" s="50"/>
       <c r="M7" s="51"/>
     </row>
     <row r="8" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="119" t="s">
+      <c r="A8" s="114" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="166" t="s">
+      <c r="B8" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="C8" s="169" t="s">
+      <c r="C8" s="122" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="119" t="s">
+      <c r="D8" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="119">
+      <c r="E8" s="114">
         <v>2</v>
       </c>
       <c r="F8" s="58" t="s">
@@ -6788,16 +7221,16 @@
       <c r="L8" s="2">
         <v>3</v>
       </c>
-      <c r="M8" s="119" t="s">
+      <c r="M8" s="114" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="120"/>
-      <c r="B9" s="167"/>
-      <c r="C9" s="170"/>
-      <c r="D9" s="120"/>
-      <c r="E9" s="120"/>
+      <c r="A9" s="115"/>
+      <c r="B9" s="120"/>
+      <c r="C9" s="123"/>
+      <c r="D9" s="115"/>
+      <c r="E9" s="115"/>
       <c r="F9" s="47" t="s">
         <v>58</v>
       </c>
@@ -6817,14 +7250,14 @@
       <c r="L9" s="2">
         <v>2</v>
       </c>
-      <c r="M9" s="120"/>
+      <c r="M9" s="115"/>
     </row>
     <row r="10" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="120"/>
-      <c r="B10" s="167"/>
-      <c r="C10" s="170"/>
-      <c r="D10" s="120"/>
-      <c r="E10" s="120"/>
+      <c r="A10" s="115"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="123"/>
+      <c r="D10" s="115"/>
+      <c r="E10" s="115"/>
       <c r="F10" s="47" t="s">
         <v>84</v>
       </c>
@@ -6844,14 +7277,14 @@
       <c r="L10" s="2">
         <v>3</v>
       </c>
-      <c r="M10" s="120"/>
+      <c r="M10" s="115"/>
     </row>
     <row r="11" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="120"/>
-      <c r="B11" s="167"/>
-      <c r="C11" s="170"/>
-      <c r="D11" s="120"/>
-      <c r="E11" s="120"/>
+      <c r="A11" s="115"/>
+      <c r="B11" s="120"/>
+      <c r="C11" s="123"/>
+      <c r="D11" s="115"/>
+      <c r="E11" s="115"/>
       <c r="F11" s="48" t="s">
         <v>52</v>
       </c>
@@ -6873,14 +7306,14 @@
       <c r="L11" s="2">
         <v>3</v>
       </c>
-      <c r="M11" s="120"/>
+      <c r="M11" s="115"/>
     </row>
     <row r="12" spans="1:13" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="121"/>
-      <c r="B12" s="168"/>
-      <c r="C12" s="171"/>
-      <c r="D12" s="121"/>
-      <c r="E12" s="121"/>
+      <c r="A12" s="116"/>
+      <c r="B12" s="121"/>
+      <c r="C12" s="124"/>
+      <c r="D12" s="116"/>
+      <c r="E12" s="116"/>
       <c r="F12" s="58" t="s">
         <v>52</v>
       </c>
@@ -6896,7 +7329,7 @@
       <c r="L12" s="5">
         <v>11</v>
       </c>
-      <c r="M12" s="121"/>
+      <c r="M12" s="116"/>
     </row>
     <row r="13" spans="1:13" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
@@ -6908,33 +7341,33 @@
       <c r="C13" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="122" t="s">
+      <c r="D13" s="117" t="s">
         <v>88</v>
       </c>
-      <c r="E13" s="123"/>
-      <c r="F13" s="123"/>
-      <c r="G13" s="123"/>
-      <c r="H13" s="123"/>
-      <c r="I13" s="123"/>
+      <c r="E13" s="118"/>
+      <c r="F13" s="118"/>
+      <c r="G13" s="118"/>
+      <c r="H13" s="118"/>
+      <c r="I13" s="118"/>
       <c r="J13" s="50"/>
       <c r="K13" s="50"/>
       <c r="L13" s="50"/>
       <c r="M13" s="51"/>
     </row>
     <row r="14" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="154" t="s">
+      <c r="A14" s="134" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="157" t="s">
+      <c r="B14" s="137" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="160" t="s">
+      <c r="C14" s="140" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="133" t="s">
+      <c r="D14" s="167" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="136">
+      <c r="E14" s="170">
         <v>1</v>
       </c>
       <c r="F14" s="58" t="s">
@@ -6957,16 +7390,16 @@
         <f>K14*E14</f>
         <v>1</v>
       </c>
-      <c r="M14" s="139" t="s">
+      <c r="M14" s="173" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="155"/>
-      <c r="B15" s="158"/>
-      <c r="C15" s="161"/>
-      <c r="D15" s="134"/>
-      <c r="E15" s="137"/>
+      <c r="A15" s="135"/>
+      <c r="B15" s="138"/>
+      <c r="C15" s="141"/>
+      <c r="D15" s="168"/>
+      <c r="E15" s="171"/>
       <c r="F15" s="47" t="s">
         <v>64</v>
       </c>
@@ -6987,21 +7420,23 @@
         <f>K15*E14</f>
         <v>0</v>
       </c>
-      <c r="M15" s="140"/>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="155"/>
-      <c r="B16" s="158"/>
-      <c r="C16" s="161"/>
-      <c r="D16" s="134"/>
-      <c r="E16" s="137"/>
+      <c r="M15" s="174"/>
+    </row>
+    <row r="16" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="135"/>
+      <c r="B16" s="138"/>
+      <c r="C16" s="141"/>
+      <c r="D16" s="168"/>
+      <c r="E16" s="171"/>
       <c r="F16" s="47" t="s">
-        <v>52</v>
+        <v>119</v>
       </c>
       <c r="G16" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="H16" s="17"/>
+        <v>79</v>
+      </c>
+      <c r="H16" s="89" t="s">
+        <v>61</v>
+      </c>
       <c r="J16" s="12" t="s">
         <v>13</v>
       </c>
@@ -7012,26 +7447,20 @@
         <f>K16*E14</f>
         <v>2</v>
       </c>
-      <c r="M16" s="140"/>
-    </row>
-    <row r="17" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="155"/>
-      <c r="B17" s="158"/>
-      <c r="C17" s="161"/>
-      <c r="D17" s="134"/>
-      <c r="E17" s="137"/>
+      <c r="M16" s="174"/>
+    </row>
+    <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="135"/>
+      <c r="B17" s="138"/>
+      <c r="C17" s="141"/>
+      <c r="D17" s="168"/>
+      <c r="E17" s="171"/>
       <c r="F17" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="60" t="s">
-        <v>78</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="I17" s="17" t="s">
-        <v>65</v>
-      </c>
+      <c r="G17" s="60"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
       <c r="J17" s="12" t="s">
         <v>14</v>
       </c>
@@ -7042,14 +7471,14 @@
         <f>K17*E14</f>
         <v>3</v>
       </c>
-      <c r="M17" s="140"/>
+      <c r="M17" s="174"/>
     </row>
     <row r="18" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="156"/>
-      <c r="B18" s="159"/>
-      <c r="C18" s="162"/>
-      <c r="D18" s="135"/>
-      <c r="E18" s="138"/>
+      <c r="A18" s="136"/>
+      <c r="B18" s="139"/>
+      <c r="C18" s="142"/>
+      <c r="D18" s="169"/>
+      <c r="E18" s="172"/>
       <c r="F18" s="58" t="s">
         <v>52</v>
       </c>
@@ -7066,7 +7495,7 @@
         <f>SUM(L14:L17)</f>
         <v>6</v>
       </c>
-      <c r="M18" s="141"/>
+      <c r="M18" s="175"/>
     </row>
     <row r="19" spans="1:16" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
@@ -7078,33 +7507,33 @@
       <c r="C19" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="122" t="s">
+      <c r="D19" s="117" t="s">
         <v>87</v>
       </c>
-      <c r="E19" s="123"/>
-      <c r="F19" s="123"/>
-      <c r="G19" s="123"/>
-      <c r="H19" s="123"/>
-      <c r="I19" s="123"/>
+      <c r="E19" s="118"/>
+      <c r="F19" s="118"/>
+      <c r="G19" s="118"/>
+      <c r="H19" s="118"/>
+      <c r="I19" s="118"/>
       <c r="J19" s="50"/>
       <c r="K19" s="50"/>
       <c r="L19" s="50"/>
       <c r="M19" s="51"/>
     </row>
     <row r="20" spans="1:16" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="163" t="s">
+      <c r="A20" s="143" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="165" t="s">
+      <c r="B20" s="145" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="108" t="s">
+      <c r="C20" s="146" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="107" t="s">
+      <c r="D20" s="147" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="110">
+      <c r="E20" s="149">
         <v>3</v>
       </c>
       <c r="F20" s="58" t="s">
@@ -7124,16 +7553,16 @@
       <c r="L20" s="5">
         <v>6</v>
       </c>
-      <c r="M20" s="130" t="s">
+      <c r="M20" s="164" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="164"/>
-      <c r="B21" s="165"/>
-      <c r="C21" s="108"/>
-      <c r="D21" s="108"/>
-      <c r="E21" s="111"/>
+      <c r="A21" s="144"/>
+      <c r="B21" s="145"/>
+      <c r="C21" s="146"/>
+      <c r="D21" s="146"/>
+      <c r="E21" s="150"/>
       <c r="F21" s="47" t="s">
         <v>66</v>
       </c>
@@ -7151,14 +7580,14 @@
       <c r="L21" s="5">
         <v>6</v>
       </c>
-      <c r="M21" s="131"/>
+      <c r="M21" s="165"/>
     </row>
     <row r="22" spans="1:16" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="164"/>
-      <c r="B22" s="165"/>
-      <c r="C22" s="108"/>
-      <c r="D22" s="108"/>
-      <c r="E22" s="111"/>
+      <c r="A22" s="144"/>
+      <c r="B22" s="145"/>
+      <c r="C22" s="146"/>
+      <c r="D22" s="146"/>
+      <c r="E22" s="150"/>
       <c r="F22" s="47" t="s">
         <v>67</v>
       </c>
@@ -7176,14 +7605,14 @@
       <c r="L22" s="5">
         <v>6</v>
       </c>
-      <c r="M22" s="131"/>
+      <c r="M22" s="165"/>
     </row>
     <row r="23" spans="1:16" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="164"/>
-      <c r="B23" s="165"/>
-      <c r="C23" s="108"/>
-      <c r="D23" s="108"/>
-      <c r="E23" s="111"/>
+      <c r="A23" s="144"/>
+      <c r="B23" s="145"/>
+      <c r="C23" s="146"/>
+      <c r="D23" s="146"/>
+      <c r="E23" s="150"/>
       <c r="F23" s="48" t="s">
         <v>52</v>
       </c>
@@ -7203,14 +7632,14 @@
       <c r="L23" s="5">
         <v>6</v>
       </c>
-      <c r="M23" s="131"/>
+      <c r="M23" s="165"/>
     </row>
     <row r="24" spans="1:16" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="164"/>
-      <c r="B24" s="165"/>
-      <c r="C24" s="108"/>
-      <c r="D24" s="109"/>
-      <c r="E24" s="112"/>
+      <c r="A24" s="144"/>
+      <c r="B24" s="145"/>
+      <c r="C24" s="146"/>
+      <c r="D24" s="148"/>
+      <c r="E24" s="151"/>
       <c r="F24" s="58" t="s">
         <v>52</v>
       </c>
@@ -7228,7 +7657,7 @@
       <c r="L24" s="5">
         <v>24</v>
       </c>
-      <c r="M24" s="132"/>
+      <c r="M24" s="166"/>
     </row>
     <row r="25" spans="1:16" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
@@ -7240,36 +7669,36 @@
       <c r="C25" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="142" t="s">
+      <c r="D25" s="176" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="143"/>
-      <c r="F25" s="143"/>
-      <c r="G25" s="143"/>
-      <c r="H25" s="143"/>
-      <c r="I25" s="143"/>
-      <c r="J25" s="143"/>
-      <c r="K25" s="143"/>
-      <c r="L25" s="143"/>
-      <c r="M25" s="144"/>
+      <c r="E25" s="177"/>
+      <c r="F25" s="177"/>
+      <c r="G25" s="177"/>
+      <c r="H25" s="177"/>
+      <c r="I25" s="177"/>
+      <c r="J25" s="177"/>
+      <c r="K25" s="177"/>
+      <c r="L25" s="177"/>
+      <c r="M25" s="178"/>
       <c r="N25" s="25"/>
       <c r="O25" s="25"/>
       <c r="P25" s="25"/>
     </row>
     <row r="26" spans="1:16" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="145" t="s">
+      <c r="A26" s="125" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="148" t="s">
+      <c r="B26" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="151" t="s">
+      <c r="C26" s="131" t="s">
         <v>91</v>
       </c>
-      <c r="D26" s="124" t="s">
+      <c r="D26" s="158" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="127">
+      <c r="E26" s="161">
         <v>3</v>
       </c>
       <c r="F26" s="58" t="s">
@@ -7290,7 +7719,7 @@
         <f>E26*K26</f>
         <v>9</v>
       </c>
-      <c r="M26" s="113" t="s">
+      <c r="M26" s="152" t="s">
         <v>17</v>
       </c>
       <c r="N26" s="25"/>
@@ -7298,11 +7727,11 @@
       <c r="P26" s="25"/>
     </row>
     <row r="27" spans="1:16" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="146"/>
-      <c r="B27" s="149"/>
-      <c r="C27" s="152"/>
-      <c r="D27" s="125"/>
-      <c r="E27" s="128"/>
+      <c r="A27" s="126"/>
+      <c r="B27" s="129"/>
+      <c r="C27" s="132"/>
+      <c r="D27" s="159"/>
+      <c r="E27" s="162"/>
       <c r="F27" s="47" t="s">
         <v>69</v>
       </c>
@@ -7321,14 +7750,14 @@
         <f>E26*K27</f>
         <v>6</v>
       </c>
-      <c r="M27" s="114"/>
+      <c r="M27" s="153"/>
     </row>
     <row r="28" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="146"/>
-      <c r="B28" s="149"/>
-      <c r="C28" s="152"/>
-      <c r="D28" s="125"/>
-      <c r="E28" s="128"/>
+      <c r="A28" s="126"/>
+      <c r="B28" s="129"/>
+      <c r="C28" s="132"/>
+      <c r="D28" s="159"/>
+      <c r="E28" s="162"/>
       <c r="F28" s="47" t="s">
         <v>52</v>
       </c>
@@ -7349,14 +7778,14 @@
         <f>E26*K28</f>
         <v>9</v>
       </c>
-      <c r="M28" s="114"/>
+      <c r="M28" s="153"/>
     </row>
     <row r="29" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="146"/>
-      <c r="B29" s="149"/>
-      <c r="C29" s="152"/>
-      <c r="D29" s="125"/>
-      <c r="E29" s="128"/>
+      <c r="A29" s="126"/>
+      <c r="B29" s="129"/>
+      <c r="C29" s="132"/>
+      <c r="D29" s="159"/>
+      <c r="E29" s="162"/>
       <c r="F29" s="48" t="s">
         <v>52</v>
       </c>
@@ -7377,14 +7806,14 @@
         <f>E26*K29</f>
         <v>9</v>
       </c>
-      <c r="M29" s="114"/>
+      <c r="M29" s="153"/>
     </row>
     <row r="30" spans="1:16" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="147"/>
-      <c r="B30" s="150"/>
-      <c r="C30" s="153"/>
-      <c r="D30" s="126"/>
-      <c r="E30" s="129"/>
+      <c r="A30" s="127"/>
+      <c r="B30" s="130"/>
+      <c r="C30" s="133"/>
+      <c r="D30" s="160"/>
+      <c r="E30" s="163"/>
       <c r="F30" s="58" t="s">
         <v>52</v>
       </c>
@@ -7401,7 +7830,7 @@
         <f>SUM(L26:L29)</f>
         <v>33</v>
       </c>
-      <c r="M30" s="115"/>
+      <c r="M30" s="154"/>
     </row>
     <row r="31" spans="1:16" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="22" t="s">
@@ -7413,42 +7842,21 @@
       <c r="C31" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="116" t="s">
+      <c r="D31" s="155" t="s">
         <v>90</v>
       </c>
-      <c r="E31" s="117"/>
-      <c r="F31" s="117"/>
-      <c r="G31" s="117"/>
-      <c r="H31" s="117"/>
-      <c r="I31" s="117"/>
-      <c r="J31" s="117"/>
-      <c r="K31" s="117"/>
-      <c r="L31" s="117"/>
-      <c r="M31" s="118"/>
+      <c r="E31" s="156"/>
+      <c r="F31" s="156"/>
+      <c r="G31" s="156"/>
+      <c r="H31" s="156"/>
+      <c r="I31" s="156"/>
+      <c r="J31" s="156"/>
+      <c r="K31" s="156"/>
+      <c r="L31" s="156"/>
+      <c r="M31" s="157"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="M2:M6"/>
-    <mergeCell ref="D7:I7"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="E2:E6"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="E8:E12"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="C26:C30"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="C20:C24"/>
     <mergeCell ref="D20:D24"/>
     <mergeCell ref="E20:E24"/>
     <mergeCell ref="M26:M30"/>
@@ -7463,6 +7871,27 @@
     <mergeCell ref="E14:E18"/>
     <mergeCell ref="M14:M18"/>
     <mergeCell ref="D25:M25"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="C26:C30"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="C20:C24"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="E8:E12"/>
+    <mergeCell ref="M2:M6"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="E2:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7538,11 +7967,11 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="str">
+      <c r="A2" s="95" t="str">
         <f>'Detalles plan de riesgo'!A2:A6</f>
         <v>R3</v>
       </c>
-      <c r="B2" s="91" t="str">
+      <c r="B2" s="98" t="str">
         <f>'Detalles plan de riesgo'!B2:B6</f>
         <v>El tiempo gastado para llevar a cabo cada una de las actividades del proyecto es superior al planeado</v>
       </c>
@@ -7571,8 +8000,8 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="51" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="92"/>
+      <c r="A3" s="96"/>
+      <c r="B3" s="99"/>
       <c r="C3" s="74" t="str">
         <f>'Detalles plan de riesgo'!F3</f>
         <v xml:space="preserve">Hacer un registro continuo de tiempos por parte de cada integrante. </v>
@@ -7600,8 +8029,8 @@
       </c>
     </row>
     <row r="4" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="89"/>
-      <c r="B4" s="92"/>
+      <c r="A4" s="96"/>
+      <c r="B4" s="99"/>
       <c r="C4" s="74"/>
       <c r="D4" s="75" t="s">
         <v>104</v>
@@ -7623,8 +8052,8 @@
       <c r="O4" s="62"/>
     </row>
     <row r="5" spans="1:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="89"/>
-      <c r="B5" s="92"/>
+      <c r="A5" s="96"/>
+      <c r="B5" s="99"/>
       <c r="C5" s="74" t="str">
         <f>'Detalles plan de riesgo'!F4</f>
         <v xml:space="preserve"> </v>
@@ -7650,8 +8079,8 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="89"/>
-      <c r="B6" s="92"/>
+      <c r="A6" s="96"/>
+      <c r="B6" s="99"/>
       <c r="C6" s="74" t="str">
         <f>'Detalles plan de riesgo'!F5</f>
         <v xml:space="preserve"> </v>
@@ -7674,8 +8103,8 @@
       <c r="O6" s="62"/>
     </row>
     <row r="7" spans="1:16" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="89"/>
-      <c r="B7" s="93"/>
+      <c r="A7" s="96"/>
+      <c r="B7" s="100"/>
       <c r="C7" s="82" t="str">
         <f>'Detalles plan de riesgo'!F6</f>
         <v xml:space="preserve"> </v>
@@ -7698,13 +8127,13 @@
       <c r="O7" s="62"/>
     </row>
     <row r="8" spans="1:16" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="90"/>
-      <c r="B8" s="94" t="s">
+      <c r="A8" s="97"/>
+      <c r="B8" s="101" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="95"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="96"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="103"/>
       <c r="F8" s="72" t="s">
         <v>75</v>
       </c>
@@ -7723,10 +8152,10 @@
       <c r="O8" s="65"/>
     </row>
     <row r="9" spans="1:16" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="88" t="s">
+      <c r="A9" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="103">
+      <c r="B9" s="110">
         <f>'Detalles plan de riesgo'!B8:B12</f>
         <v>0</v>
       </c>
@@ -7749,8 +8178,8 @@
       <c r="O9" s="61"/>
     </row>
     <row r="10" spans="1:16" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="89"/>
-      <c r="B10" s="104"/>
+      <c r="A10" s="96"/>
+      <c r="B10" s="111"/>
       <c r="C10" s="74" t="str">
         <f>'Detalles plan de riesgo'!F9</f>
         <v xml:space="preserve"> Fijar reuniones semanales de seguimiento </v>
@@ -7771,8 +8200,8 @@
       <c r="O10" s="62"/>
     </row>
     <row r="11" spans="1:16" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="89"/>
-      <c r="B11" s="104"/>
+      <c r="A11" s="96"/>
+      <c r="B11" s="111"/>
       <c r="C11" s="74" t="str">
         <f>'Detalles plan de riesgo'!F10</f>
         <v>Generar archivos de seguimiento al proyecto, formatos por rol  y formato de integración de componentes</v>
@@ -7795,8 +8224,8 @@
       <c r="O11" s="62"/>
     </row>
     <row r="12" spans="1:16" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="89"/>
-      <c r="B12" s="104"/>
+      <c r="A12" s="96"/>
+      <c r="B12" s="111"/>
       <c r="C12" s="74" t="str">
         <f>'Detalles plan de riesgo'!F11</f>
         <v xml:space="preserve"> </v>
@@ -7819,8 +8248,8 @@
       <c r="O12" s="62"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="89"/>
-      <c r="B13" s="104"/>
+      <c r="A13" s="96"/>
+      <c r="B13" s="111"/>
       <c r="C13" s="74" t="str">
         <f>'Detalles plan de riesgo'!F12</f>
         <v xml:space="preserve"> </v>
@@ -7839,13 +8268,13 @@
       <c r="O13" s="62"/>
     </row>
     <row r="14" spans="1:16" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="90"/>
-      <c r="B14" s="105" t="s">
+      <c r="A14" s="97"/>
+      <c r="B14" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="106"/>
+      <c r="C14" s="100"/>
+      <c r="D14" s="100"/>
+      <c r="E14" s="113"/>
       <c r="F14" s="72" t="s">
         <v>76</v>
       </c>
@@ -7860,10 +8289,10 @@
       <c r="O14" s="65"/>
     </row>
     <row r="15" spans="1:16" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="88" t="s">
+      <c r="A15" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="103" t="s">
+      <c r="B15" s="110" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="78" t="str">
@@ -7886,8 +8315,8 @@
       <c r="O15" s="61"/>
     </row>
     <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="89"/>
-      <c r="B16" s="104"/>
+      <c r="A16" s="96"/>
+      <c r="B16" s="111"/>
       <c r="C16" s="74" t="str">
         <f>'Detalles plan de riesgo'!F15</f>
         <v xml:space="preserve"> Hacer seguimiento al uso del SVN</v>
@@ -7910,11 +8339,11 @@
       <c r="O16" s="62"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="89"/>
-      <c r="B17" s="104"/>
+      <c r="A17" s="96"/>
+      <c r="B17" s="111"/>
       <c r="C17" s="74" t="str">
         <f>'Detalles plan de riesgo'!F16</f>
-        <v xml:space="preserve"> </v>
+        <v xml:space="preserve">Realizar copias de seguridad preventivas </v>
       </c>
       <c r="D17" s="75"/>
       <c r="E17" s="81"/>
@@ -7930,15 +8359,15 @@
       <c r="O17" s="62"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="89"/>
-      <c r="B18" s="104"/>
+      <c r="A18" s="96"/>
+      <c r="B18" s="111"/>
       <c r="C18" s="74" t="str">
         <f>'Detalles plan de riesgo'!F17</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D18" s="74" t="str">
+      <c r="D18" s="74">
         <f>'Detalles plan de riesgo'!G17</f>
-        <v xml:space="preserve"> Contingencia</v>
+        <v>0</v>
       </c>
       <c r="E18" s="81"/>
       <c r="F18" s="73"/>
@@ -7953,8 +8382,8 @@
       <c r="O18" s="62"/>
     </row>
     <row r="19" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="89"/>
-      <c r="B19" s="104"/>
+      <c r="A19" s="96"/>
+      <c r="B19" s="111"/>
       <c r="C19" s="74" t="str">
         <f>'Detalles plan de riesgo'!F18</f>
         <v xml:space="preserve"> </v>
@@ -7977,13 +8406,13 @@
       <c r="O19" s="62"/>
     </row>
     <row r="20" spans="1:15" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="90"/>
-      <c r="B20" s="105" t="s">
+      <c r="A20" s="97"/>
+      <c r="B20" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="93"/>
-      <c r="D20" s="93"/>
-      <c r="E20" s="106"/>
+      <c r="C20" s="100"/>
+      <c r="D20" s="100"/>
+      <c r="E20" s="113"/>
       <c r="F20" s="65"/>
       <c r="G20" s="56"/>
       <c r="H20" s="56"/>
@@ -7996,10 +8425,10 @@
       <c r="O20" s="65"/>
     </row>
     <row r="21" spans="1:15" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="88" t="s">
+      <c r="A21" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="103" t="s">
+      <c r="B21" s="110" t="s">
         <v>51</v>
       </c>
       <c r="C21" s="78" t="str">
@@ -8024,8 +8453,8 @@
       <c r="O21" s="61"/>
     </row>
     <row r="22" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A22" s="89"/>
-      <c r="B22" s="104"/>
+      <c r="A22" s="96"/>
+      <c r="B22" s="111"/>
       <c r="C22" s="74" t="str">
         <f>'Detalles plan de riesgo'!F21</f>
         <v>Realizar pruebas iniciales con datos de ejemplo para identificar alcance</v>
@@ -8048,8 +8477,8 @@
       <c r="O22" s="62"/>
     </row>
     <row r="23" spans="1:15" ht="51" x14ac:dyDescent="0.25">
-      <c r="A23" s="89"/>
-      <c r="B23" s="104"/>
+      <c r="A23" s="96"/>
+      <c r="B23" s="111"/>
       <c r="C23" s="74" t="str">
         <f>'Detalles plan de riesgo'!F22</f>
         <v xml:space="preserve"> 2 personas deben conocer de un componente tecnologico </v>
@@ -8070,8 +8499,8 @@
       <c r="O23" s="62"/>
     </row>
     <row r="24" spans="1:15" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="89"/>
-      <c r="B24" s="104"/>
+      <c r="A24" s="96"/>
+      <c r="B24" s="111"/>
       <c r="C24" s="74" t="str">
         <f>'Detalles plan de riesgo'!F23</f>
         <v xml:space="preserve"> </v>
@@ -8094,8 +8523,8 @@
       <c r="O24" s="62"/>
     </row>
     <row r="25" spans="1:15" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="89"/>
-      <c r="B25" s="104"/>
+      <c r="A25" s="96"/>
+      <c r="B25" s="111"/>
       <c r="C25" s="74" t="str">
         <f>'Detalles plan de riesgo'!F24</f>
         <v xml:space="preserve"> </v>
@@ -8118,11 +8547,11 @@
       <c r="O25" s="62"/>
     </row>
     <row r="26" spans="1:15" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="90"/>
-      <c r="B26" s="105" t="s">
+      <c r="A26" s="97"/>
+      <c r="B26" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="93"/>
+      <c r="C26" s="100"/>
       <c r="D26" s="85"/>
       <c r="E26" s="83"/>
       <c r="F26" s="65"/>
@@ -8137,10 +8566,10 @@
       <c r="O26" s="65"/>
     </row>
     <row r="27" spans="1:15" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="88" t="s">
+      <c r="A27" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="103" t="s">
+      <c r="B27" s="110" t="s">
         <v>33</v>
       </c>
       <c r="C27" s="78" t="str">
@@ -8165,8 +8594,8 @@
       <c r="O27" s="61"/>
     </row>
     <row r="28" spans="1:15" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="89"/>
-      <c r="B28" s="104"/>
+      <c r="A28" s="96"/>
+      <c r="B28" s="111"/>
       <c r="C28" s="74" t="str">
         <f>'Detalles plan de riesgo'!F27</f>
         <v>Si un miembro sabe que no va a estar disponible en una fecha dada, que en lo posible adelante su aporte al trabajo grupal</v>
@@ -8189,8 +8618,8 @@
       <c r="O28" s="62"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="89"/>
-      <c r="B29" s="104"/>
+      <c r="A29" s="96"/>
+      <c r="B29" s="111"/>
       <c r="C29" s="74" t="str">
         <f>'Detalles plan de riesgo'!F28</f>
         <v xml:space="preserve"> </v>
@@ -8213,8 +8642,8 @@
       <c r="O29" s="62"/>
     </row>
     <row r="30" spans="1:15" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="89"/>
-      <c r="B30" s="104"/>
+      <c r="A30" s="96"/>
+      <c r="B30" s="111"/>
       <c r="C30" s="74" t="str">
         <f>'Detalles plan de riesgo'!F29</f>
         <v xml:space="preserve"> </v>
@@ -8237,8 +8666,8 @@
       <c r="O30" s="62"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="89"/>
-      <c r="B31" s="104"/>
+      <c r="A31" s="96"/>
+      <c r="B31" s="111"/>
       <c r="C31" s="74" t="str">
         <f>'Detalles plan de riesgo'!F30</f>
         <v xml:space="preserve"> </v>
@@ -8257,11 +8686,11 @@
       <c r="O31" s="62"/>
     </row>
     <row r="32" spans="1:15" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="90"/>
-      <c r="B32" s="105" t="s">
+      <c r="A32" s="97"/>
+      <c r="B32" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="93"/>
+      <c r="C32" s="100"/>
       <c r="D32" s="84"/>
       <c r="E32" s="83"/>
       <c r="F32" s="65"/>
@@ -8294,302 +8723,302 @@
     <mergeCell ref="B14:E14"/>
   </mergeCells>
   <conditionalFormatting sqref="G2:O7 D2:D4 F8:O8">
-    <cfRule type="cellIs" dxfId="69" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="77" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="78" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13 H12:O12 H18:O19 D24:D25 H24:O25 F31 H29:O31 D29:D30 G9:O11 G21:O23 G27:O28 F13:O14">
-    <cfRule type="cellIs" dxfId="67" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="75" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="76" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:O20">
-    <cfRule type="cellIs" dxfId="65" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="73" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="74" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26 F26:O26">
-    <cfRule type="cellIs" dxfId="63" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="71" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="72" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F32:O32">
-    <cfRule type="cellIs" dxfId="61" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="69" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="70" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2 D13 H12:O12 H18:O19 D24:D25 H24:O25 F31 H29:O31 D29:D30 G2:O4 G9:O11 G21:O23 G27:O28 F13:O13">
-    <cfRule type="cellIs" dxfId="59" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="66" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D4">
-    <cfRule type="cellIs" dxfId="58" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="65" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:O7">
-    <cfRule type="cellIs" dxfId="57" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="64" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15:O17">
-    <cfRule type="cellIs" dxfId="56" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="59" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="60" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15:O17">
-    <cfRule type="cellIs" dxfId="54" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="58" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="cellIs" dxfId="53" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="53" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="54" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="cellIs" dxfId="51" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="52" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="cellIs" dxfId="50" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="50" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="51" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="cellIs" dxfId="48" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="49" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18:G19">
-    <cfRule type="cellIs" dxfId="47" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="47" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="48" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18:G19">
-    <cfRule type="cellIs" dxfId="45" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="46" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G24:G25">
-    <cfRule type="cellIs" dxfId="44" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="44" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="45" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G24:G25">
-    <cfRule type="cellIs" dxfId="42" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="43" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29:G31">
-    <cfRule type="cellIs" dxfId="41" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="41" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="42" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29:G31">
-    <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="40" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F7">
-    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="38" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="39" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="36" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="37" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F4">
-    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="36" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F7">
-    <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="35" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9:F11">
-    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="33" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="34" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9:F11">
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="32" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="30" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="31" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="29" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="27" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="28" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="26" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21:F23">
-    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="24" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="25" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21:F23">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="23" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24:F25">
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="21" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="22" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24:F25">
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="20" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27:F28">
-    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="18" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="19" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27:F28">
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="17" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29:F30">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="15" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="16" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F29:F30">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="14" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9:D11">
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="12" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="13" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15:D17">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="10" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="11" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:D23">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="8" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="7" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31:D32">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E7 E21:E32 E9:E13 E15:E19">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
       <formula>$P$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="3" operator="equal">
       <formula>$P$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>